<commit_message>
sblm di cek dosen
</commit_message>
<xml_diff>
--- a/Dokumen Pendukung/analisis_data.xlsx
+++ b/Dokumen Pendukung/analisis_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Skripsi\Dokumen Pendukung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A960AE16-2C7F-4F6E-A0A5-CF37C9216701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F572AE-2A52-4EA1-A7ED-FBD577EACEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A5405BB2-1FC9-49C8-AA96-A8AB9CA15270}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="48">
   <si>
     <t>Ukuran Data</t>
   </si>
@@ -123,12 +124,69 @@
   <si>
     <t>Keberhasilan</t>
   </si>
+  <si>
+    <t>Shannon Entropy</t>
+  </si>
+  <si>
+    <t>Max Entropy</t>
+  </si>
+  <si>
+    <t>Randomness Percentage</t>
+  </si>
+  <si>
+    <t>Chi-Square Statistic</t>
+  </si>
+  <si>
+    <t>Passes Test</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>61.72%</t>
+  </si>
+  <si>
+    <t>0.7415</t>
+  </si>
+  <si>
+    <t>Uniform</t>
+  </si>
+  <si>
+    <t>67.96%</t>
+  </si>
+  <si>
+    <t>232.26</t>
+  </si>
+  <si>
+    <t>0.8435</t>
+  </si>
+  <si>
+    <t>58.70%</t>
+  </si>
+  <si>
+    <t>331.61</t>
+  </si>
+  <si>
+    <t>0.0009</t>
+  </si>
+  <si>
+    <t>Non-uniform</t>
+  </si>
+  <si>
+    <t>68.25%</t>
+  </si>
+  <si>
+    <t>P-Value</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +277,66 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,8 +361,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBDBDB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DB3E2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6D9F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -393,11 +539,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -415,6 +626,81 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,70 +737,88 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="16" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -867,7 +1171,7 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="32" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -884,7 +1188,7 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="32"/>
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
@@ -901,7 +1205,7 @@
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
@@ -918,11 +1222,11 @@
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="32"/>
+      <c r="F5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="34">
         <v>3.8189999999999999E-3</v>
       </c>
     </row>
@@ -930,17 +1234,17 @@
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="1"/>
       <c r="I7" s="3"/>
     </row>
@@ -948,7 +1252,7 @@
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="32" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -962,7 +1266,7 @@
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
@@ -974,7 +1278,7 @@
       <c r="A10">
         <v>10</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="4" t="s">
         <v>7</v>
       </c>
@@ -986,11 +1290,11 @@
       <c r="A11">
         <v>11</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="32"/>
+      <c r="F11" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="34">
         <v>6.6889999999999996E-3</v>
       </c>
     </row>
@@ -998,17 +1302,17 @@
       <c r="A12">
         <v>12</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1048,7 +1352,7 @@
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="32" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1064,7 +1368,7 @@
       <c r="A19">
         <v>19</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="32"/>
       <c r="F19" s="4" t="s">
         <v>6</v>
       </c>
@@ -1078,7 +1382,7 @@
       <c r="A20">
         <v>20</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="32"/>
       <c r="F20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1090,11 +1394,11 @@
       <c r="A21">
         <v>21</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8" t="s">
+      <c r="E21" s="32"/>
+      <c r="F21" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="34">
         <v>3.8189999999999999E-3</v>
       </c>
     </row>
@@ -1102,23 +1406,23 @@
       <c r="A22">
         <v>22</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="32" t="s">
         <v>2</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -1132,7 +1436,7 @@
       <c r="A25">
         <v>25</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="32"/>
       <c r="F25" s="4" t="s">
         <v>6</v>
       </c>
@@ -1144,7 +1448,7 @@
       <c r="A26">
         <v>26</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="32"/>
       <c r="F26" s="4" t="s">
         <v>7</v>
       </c>
@@ -1158,11 +1462,11 @@
       <c r="A27">
         <v>27</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8" t="s">
+      <c r="E27" s="32"/>
+      <c r="F27" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="34">
         <v>6.5779999999999996E-3</v>
       </c>
       <c r="I27" s="2"/>
@@ -1172,9 +1476,9 @@
       <c r="A28">
         <v>28</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
@@ -1182,9 +1486,9 @@
       <c r="A29">
         <v>29</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="9"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="34"/>
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
     </row>
@@ -1220,7 +1524,7 @@
       <c r="A32">
         <v>32</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="35" t="s">
         <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
@@ -1229,7 +1533,7 @@
       <c r="G32" s="5">
         <v>6.7120000000000001E-3</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="I32" s="32" t="s">
         <v>1</v>
       </c>
       <c r="J32" s="4" t="s">
@@ -1243,14 +1547,14 @@
       <c r="A33">
         <v>33</v>
       </c>
-      <c r="E33" s="11"/>
+      <c r="E33" s="36"/>
       <c r="F33" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G33" s="5">
         <v>6.7080000000000004E-3</v>
       </c>
-      <c r="I33" s="7"/>
+      <c r="I33" s="32"/>
       <c r="J33" s="4" t="s">
         <v>6</v>
       </c>
@@ -1262,14 +1566,14 @@
       <c r="A34">
         <v>34</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="36"/>
       <c r="F34" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G34" s="5">
         <v>6.3160000000000004E-3</v>
       </c>
-      <c r="I34" s="7"/>
+      <c r="I34" s="32"/>
       <c r="J34" s="4" t="s">
         <v>7</v>
       </c>
@@ -1281,18 +1585,18 @@
       <c r="A35">
         <v>35</v>
       </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="13" t="s">
+      <c r="E35" s="36"/>
+      <c r="F35" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="16">
+      <c r="G35" s="41">
         <v>6.5779999999999996E-3</v>
       </c>
-      <c r="I35" s="7"/>
-      <c r="J35" s="8" t="s">
+      <c r="I35" s="32"/>
+      <c r="J35" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="K35" s="9">
+      <c r="K35" s="34">
         <v>3.8189999999999999E-3</v>
       </c>
     </row>
@@ -1300,29 +1604,29 @@
       <c r="A36">
         <v>36</v>
       </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="17"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="9"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="42"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="34"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="18"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="9"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="43"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="34"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="35" t="s">
         <v>2</v>
       </c>
       <c r="F38" s="4" t="s">
@@ -1331,7 +1635,7 @@
       <c r="G38" s="5">
         <v>3.8070000000000001E-3</v>
       </c>
-      <c r="I38" s="7" t="s">
+      <c r="I38" s="32" t="s">
         <v>2</v>
       </c>
       <c r="J38" s="4" t="s">
@@ -1345,14 +1649,14 @@
       <c r="A39">
         <v>39</v>
       </c>
-      <c r="E39" s="11"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G39" s="5">
         <v>3.8070000000000001E-3</v>
       </c>
-      <c r="I39" s="7"/>
+      <c r="I39" s="32"/>
       <c r="J39" s="4" t="s">
         <v>6</v>
       </c>
@@ -1364,14 +1668,14 @@
       <c r="A40">
         <v>40</v>
       </c>
-      <c r="E40" s="11"/>
+      <c r="E40" s="36"/>
       <c r="F40" s="4" t="s">
         <v>7</v>
       </c>
       <c r="G40" s="5">
         <v>3.8070000000000001E-3</v>
       </c>
-      <c r="I40" s="7"/>
+      <c r="I40" s="32"/>
       <c r="J40" s="4" t="s">
         <v>7</v>
       </c>
@@ -1383,18 +1687,18 @@
       <c r="A41">
         <v>41</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="13" t="s">
+      <c r="E41" s="36"/>
+      <c r="F41" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="16">
+      <c r="G41" s="41">
         <v>3.8070000000000001E-3</v>
       </c>
-      <c r="I41" s="7"/>
-      <c r="J41" s="8" t="s">
+      <c r="I41" s="32"/>
+      <c r="J41" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="K41" s="9">
+      <c r="K41" s="34">
         <v>6.5779999999999996E-3</v>
       </c>
     </row>
@@ -1402,23 +1706,23 @@
       <c r="A42">
         <v>42</v>
       </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="17"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="9"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="42"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="34"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="18"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="9"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="43"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="34"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -1448,7 +1752,7 @@
       <c r="A47">
         <v>47</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="32" t="s">
         <v>1</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -1462,7 +1766,7 @@
       <c r="A48">
         <v>48</v>
       </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="32"/>
       <c r="F48" s="4" t="s">
         <v>6</v>
       </c>
@@ -1474,7 +1778,7 @@
       <c r="A49">
         <v>49</v>
       </c>
-      <c r="E49" s="7"/>
+      <c r="E49" s="32"/>
       <c r="F49" s="4" t="s">
         <v>7</v>
       </c>
@@ -1486,11 +1790,11 @@
       <c r="A50">
         <v>50</v>
       </c>
-      <c r="E50" s="7"/>
-      <c r="F50" s="8" t="s">
+      <c r="E50" s="32"/>
+      <c r="F50" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="34">
         <v>6.6889999999999996E-3</v>
       </c>
     </row>
@@ -1498,23 +1802,23 @@
       <c r="A51">
         <v>51</v>
       </c>
-      <c r="E51" s="7"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="9"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="34"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>52</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="9"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="32" t="s">
         <v>2</v>
       </c>
       <c r="F53" s="4" t="s">
@@ -1528,7 +1832,7 @@
       <c r="A54">
         <v>54</v>
       </c>
-      <c r="E54" s="7"/>
+      <c r="E54" s="32"/>
       <c r="F54" s="4" t="s">
         <v>6</v>
       </c>
@@ -1540,7 +1844,7 @@
       <c r="A55">
         <v>55</v>
       </c>
-      <c r="E55" s="7"/>
+      <c r="E55" s="32"/>
       <c r="F55" s="4" t="s">
         <v>7</v>
       </c>
@@ -1552,11 +1856,11 @@
       <c r="A56">
         <v>56</v>
       </c>
-      <c r="E56" s="7"/>
-      <c r="F56" s="8" t="s">
+      <c r="E56" s="32"/>
+      <c r="F56" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="34">
         <v>3.8189999999999999E-3</v>
       </c>
     </row>
@@ -1564,17 +1868,17 @@
       <c r="A57">
         <v>57</v>
       </c>
-      <c r="E57" s="7"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="9"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="34"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>58</v>
       </c>
-      <c r="E58" s="7"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="9"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="34"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -1607,7 +1911,7 @@
       <c r="A62">
         <v>62</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="32" t="s">
         <v>1</v>
       </c>
       <c r="F62" s="4" t="s">
@@ -1621,7 +1925,7 @@
       <c r="A63">
         <v>63</v>
       </c>
-      <c r="E63" s="7"/>
+      <c r="E63" s="32"/>
       <c r="F63" s="4" t="s">
         <v>6</v>
       </c>
@@ -1633,7 +1937,7 @@
       <c r="A64">
         <v>64</v>
       </c>
-      <c r="E64" s="7"/>
+      <c r="E64" s="32"/>
       <c r="F64" s="4" t="s">
         <v>7</v>
       </c>
@@ -1645,11 +1949,11 @@
       <c r="A65">
         <v>65</v>
       </c>
-      <c r="E65" s="7"/>
-      <c r="F65" s="8" t="s">
+      <c r="E65" s="32"/>
+      <c r="F65" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G65" s="9">
+      <c r="G65" s="34">
         <v>4.9433999999999999E-2</v>
       </c>
     </row>
@@ -1657,23 +1961,23 @@
       <c r="A66">
         <v>66</v>
       </c>
-      <c r="E66" s="7"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="9"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="34"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>67</v>
       </c>
-      <c r="E67" s="7"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="9"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="34"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>68</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E68" s="32" t="s">
         <v>2</v>
       </c>
       <c r="F68" s="4" t="s">
@@ -1687,7 +1991,7 @@
       <c r="A69">
         <v>69</v>
       </c>
-      <c r="E69" s="7"/>
+      <c r="E69" s="32"/>
       <c r="F69" s="4" t="s">
         <v>6</v>
       </c>
@@ -1699,7 +2003,7 @@
       <c r="A70">
         <v>70</v>
       </c>
-      <c r="E70" s="7"/>
+      <c r="E70" s="32"/>
       <c r="F70" s="4" t="s">
         <v>7</v>
       </c>
@@ -1711,11 +2015,11 @@
       <c r="A71">
         <v>71</v>
       </c>
-      <c r="E71" s="7"/>
-      <c r="F71" s="8" t="s">
+      <c r="E71" s="32"/>
+      <c r="F71" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G71" s="9">
+      <c r="G71" s="34">
         <v>2.8087000000000001E-2</v>
       </c>
     </row>
@@ -1723,17 +2027,17 @@
       <c r="A72">
         <v>72</v>
       </c>
-      <c r="E72" s="7"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="9"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="34"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>73</v>
       </c>
-      <c r="E73" s="7"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="9"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="34"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -1771,7 +2075,7 @@
       <c r="A78">
         <v>78</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="E78" s="32" t="s">
         <v>1</v>
       </c>
       <c r="F78" s="4" t="s">
@@ -1785,7 +2089,7 @@
       <c r="A79">
         <v>79</v>
       </c>
-      <c r="E79" s="7"/>
+      <c r="E79" s="32"/>
       <c r="F79" s="4" t="s">
         <v>6</v>
       </c>
@@ -1797,7 +2101,7 @@
       <c r="A80">
         <v>80</v>
       </c>
-      <c r="E80" s="7"/>
+      <c r="E80" s="32"/>
       <c r="F80" s="4" t="s">
         <v>7</v>
       </c>
@@ -1809,11 +2113,11 @@
       <c r="A81">
         <v>81</v>
       </c>
-      <c r="E81" s="7"/>
-      <c r="F81" s="8" t="s">
+      <c r="E81" s="32"/>
+      <c r="F81" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G81" s="9">
+      <c r="G81" s="34">
         <v>4.6383000000000001E-2</v>
       </c>
     </row>
@@ -1821,23 +2125,23 @@
       <c r="A82">
         <v>82</v>
       </c>
-      <c r="E82" s="7"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="9"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="34"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>83</v>
       </c>
-      <c r="E83" s="7"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="9"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="34"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>84</v>
       </c>
-      <c r="E84" s="7" t="s">
+      <c r="E84" s="32" t="s">
         <v>2</v>
       </c>
       <c r="F84" s="4" t="s">
@@ -1851,7 +2155,7 @@
       <c r="A85">
         <v>85</v>
       </c>
-      <c r="E85" s="7"/>
+      <c r="E85" s="32"/>
       <c r="F85" s="4" t="s">
         <v>6</v>
       </c>
@@ -1863,7 +2167,7 @@
       <c r="A86">
         <v>86</v>
       </c>
-      <c r="E86" s="7"/>
+      <c r="E86" s="32"/>
       <c r="F86" s="4" t="s">
         <v>7</v>
       </c>
@@ -1875,11 +2179,11 @@
       <c r="A87">
         <v>87</v>
       </c>
-      <c r="E87" s="7"/>
-      <c r="F87" s="8" t="s">
+      <c r="E87" s="32"/>
+      <c r="F87" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G87" s="9">
+      <c r="G87" s="34">
         <v>2.4201E-2</v>
       </c>
     </row>
@@ -1887,17 +2191,17 @@
       <c r="A88">
         <v>88</v>
       </c>
-      <c r="E88" s="7"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="9"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="34"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>89</v>
       </c>
-      <c r="E89" s="7"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="9"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="33"/>
+      <c r="G89" s="34"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
@@ -3506,10 +3810,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC6E717-CD80-42F9-B90A-1283E2E05531}">
-  <dimension ref="B1:L33"/>
+  <dimension ref="B1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="J2" sqref="I2:K2"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3519,465 +3823,926 @@
     <col min="4" max="4" width="8.140625" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
+    <row r="1" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:21" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="32" t="s">
+      <c r="K2" s="51"/>
+      <c r="L2" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20">
+    <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="47">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="8">
         <v>1</v>
       </c>
-      <c r="H3" s="36" t="s">
+      <c r="H3" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="33" t="s">
+      <c r="J3" s="52"/>
+      <c r="K3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="34">
+      <c r="L3" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23" t="s">
+    <row r="4" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="10">
         <v>1</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="40" t="s">
+      <c r="H4" s="45"/>
+      <c r="I4" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="33" t="s">
+      <c r="J4" s="52"/>
+      <c r="K4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="34">
+      <c r="L4" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20">
+    <row r="5" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="47">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="33" t="s">
+      <c r="J5" s="52"/>
+      <c r="K5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23" t="s">
+    <row r="6" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="H6" s="37"/>
-      <c r="I6" s="40" t="s">
+      <c r="H6" s="45"/>
+      <c r="I6" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="33" t="s">
+      <c r="J6" s="52"/>
+      <c r="K6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L6" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20">
+    <row r="7" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="47">
         <v>3</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="8">
         <v>1</v>
       </c>
-      <c r="H7" s="39" t="s">
+      <c r="H7" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="40"/>
-      <c r="K7" s="33" t="s">
+      <c r="J7" s="52"/>
+      <c r="K7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L7" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23" t="s">
+    <row r="8" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="10">
         <v>1</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="40" t="s">
+      <c r="H8" s="45"/>
+      <c r="I8" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="40"/>
-      <c r="K8" s="33" t="s">
+      <c r="J8" s="52"/>
+      <c r="K8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L8" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="25">
+    <row r="9" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="50">
         <v>4</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="40"/>
-      <c r="K9" s="33" t="s">
+      <c r="J9" s="52"/>
+      <c r="K9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23" t="s">
+    <row r="10" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="10">
         <v>1</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="40" t="s">
+      <c r="H10" s="45"/>
+      <c r="I10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="40"/>
-      <c r="K10" s="33" t="s">
+      <c r="J10" s="52"/>
+      <c r="K10" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="34">
+      <c r="L10" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="2:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26" t="s">
+    <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:21" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="27">
+    <row r="13" spans="2:21" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
         <v>1</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="12">
         <v>5</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="12">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-      <c r="C14" s="27">
+      <c r="N13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="T13" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="U13" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="12">
         <v>4</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="12">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="27">
+      <c r="N14" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="31">
+        <v>49375</v>
+      </c>
+      <c r="P14" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14" s="30">
+        <v>240</v>
+      </c>
+      <c r="S14" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="T14" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="U14" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="12">
         <v>4</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="12">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="27">
+      <c r="N15" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="O15" s="31">
+        <v>54366</v>
+      </c>
+      <c r="P15" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="S15" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="T15" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="U15" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="12">
         <v>2</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="12">
         <v>3</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="12">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29"/>
-      <c r="C17" s="30">
+      <c r="N16" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="31">
+        <v>46956</v>
+      </c>
+      <c r="P16" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="R16" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="S16" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="T16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="U16" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15">
         <v>4</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="15">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G25" s="32" t="s">
+      <c r="N17" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="31">
+        <v>54599</v>
+      </c>
+      <c r="P17" s="30">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="R17" s="30">
+        <v>240</v>
+      </c>
+      <c r="S17" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="T17" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="U17" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N20" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P20" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N21" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="23">
+        <v>49375</v>
+      </c>
+      <c r="P21" s="24">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N22" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22" s="23">
+        <v>54366</v>
+      </c>
+      <c r="P22" s="24">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="23">
+        <v>46956</v>
+      </c>
+      <c r="P23" s="24">
+        <v>8</v>
+      </c>
+      <c r="Q23" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="23">
+        <v>54599</v>
+      </c>
+      <c r="P24" s="24">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="32" t="s">
+      <c r="H25" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="I25" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="35"/>
-      <c r="K25" s="32" t="s">
+      <c r="J25" s="51"/>
+      <c r="K25" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="32" t="s">
+      <c r="L25" s="17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="36">
+      <c r="N25" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="P25" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q25" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="R25" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="46">
         <v>1</v>
       </c>
-      <c r="H26" s="36" t="s">
+      <c r="H26" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="I26" s="33" t="s">
+      <c r="I26" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="38" t="s">
+      <c r="J26" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="K26" s="38"/>
-      <c r="L26" s="34">
+      <c r="K26" s="49"/>
+      <c r="L26" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="33" t="s">
+      <c r="N26" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" s="28">
+        <v>240</v>
+      </c>
+      <c r="P26" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q26" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="R26" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="38" t="s">
+      <c r="J27" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="38"/>
-      <c r="L27" s="34">
+      <c r="K27" s="49"/>
+      <c r="L27" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G28" s="39">
+      <c r="N27" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="O27" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="P27" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q27" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="R27" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="44">
         <v>2</v>
       </c>
-      <c r="H28" s="39" t="s">
+      <c r="H28" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="33" t="s">
+      <c r="I28" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J28" s="38" t="s">
+      <c r="J28" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="K28" s="38"/>
-      <c r="L28" s="34">
+      <c r="K28" s="49"/>
+      <c r="L28" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="33" t="s">
+      <c r="N28" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O28" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="P28" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q28" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="R28" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J29" s="38" t="s">
+      <c r="J29" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="K29" s="38"/>
-      <c r="L29" s="34">
+      <c r="K29" s="49"/>
+      <c r="L29" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="39">
+      <c r="N29" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="O29" s="28">
+        <v>240</v>
+      </c>
+      <c r="P29" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q29" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="R29" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="44">
         <v>3</v>
       </c>
-      <c r="H30" s="39" t="s">
+      <c r="H30" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="I30" s="33" t="s">
+      <c r="I30" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="38" t="s">
+      <c r="J30" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="38"/>
-      <c r="L30" s="34">
+      <c r="K30" s="49"/>
+      <c r="L30" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="33" t="s">
+    <row r="31" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J31" s="38" t="s">
+      <c r="J31" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="K31" s="38"/>
-      <c r="L31" s="34">
+      <c r="K31" s="49"/>
+      <c r="L31" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="44">
+        <v>4</v>
+      </c>
+      <c r="H32" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="K32" s="49"/>
+      <c r="L32" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G32" s="39">
-        <v>4</v>
-      </c>
-      <c r="H32" s="39" t="s">
+    <row r="33" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="49"/>
+      <c r="L33" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G36" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="I36" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="J36" s="59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="57">
+        <v>49375</v>
+      </c>
+      <c r="I37" s="60">
+        <v>8</v>
+      </c>
+      <c r="J37" s="60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="53"/>
+      <c r="H38" s="55">
+        <v>54366</v>
+      </c>
+      <c r="I38" s="56">
+        <v>8</v>
+      </c>
+      <c r="J38" s="56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="55">
+        <v>46956</v>
+      </c>
+      <c r="I39" s="56">
+        <v>8</v>
+      </c>
+      <c r="J39" s="56" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="53"/>
+      <c r="H40" s="55">
+        <v>54599</v>
+      </c>
+      <c r="I40" s="56">
+        <v>8</v>
+      </c>
+      <c r="J40" s="56" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="55">
+        <v>49375</v>
+      </c>
+      <c r="I41" s="56">
+        <v>8</v>
+      </c>
+      <c r="J41" s="56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G42" s="53"/>
+      <c r="H42" s="55">
+        <v>54366</v>
+      </c>
+      <c r="I42" s="56">
+        <v>8</v>
+      </c>
+      <c r="J42" s="56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G43" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="38"/>
-      <c r="L32" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="J33" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" s="38"/>
-      <c r="L33" s="34">
-        <v>1</v>
+      <c r="H43" s="55">
+        <v>46956</v>
+      </c>
+      <c r="I43" s="56">
+        <v>8</v>
+      </c>
+      <c r="J43" s="56" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="7:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G44" s="53"/>
+      <c r="H44" s="55">
+        <v>54599</v>
+      </c>
+      <c r="I44" s="56">
+        <v>8</v>
+      </c>
+      <c r="J44" s="56" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="14:17" ht="24" x14ac:dyDescent="0.25">
+      <c r="N51" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="O51" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="P51" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q51" s="61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N52" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="O52" s="63">
+        <v>49375</v>
+      </c>
+      <c r="P52" s="62">
+        <v>8</v>
+      </c>
+      <c r="Q52" s="62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N53" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="O53" s="63">
+        <v>54366</v>
+      </c>
+      <c r="P53" s="62">
+        <v>8</v>
+      </c>
+      <c r="Q53" s="62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N54" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="O54" s="63">
+        <v>46956</v>
+      </c>
+      <c r="P54" s="62">
+        <v>8</v>
+      </c>
+      <c r="Q54" s="62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N55" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="O55" s="63">
+        <v>54599</v>
+      </c>
+      <c r="P55" s="62">
+        <v>8</v>
+      </c>
+      <c r="Q55" s="62" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="42">
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:J7"/>
@@ -4016,6 +4781,315 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="G41:G42"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DF5B10-5821-4AE1-B9F6-73B5D5089F46}">
+  <dimension ref="A2:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="2" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="63">
+        <v>49375</v>
+      </c>
+      <c r="C3" s="62">
+        <v>8</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="63">
+        <v>54366</v>
+      </c>
+      <c r="C4" s="62">
+        <v>8</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="63">
+        <v>46956</v>
+      </c>
+      <c r="C5" s="62">
+        <v>8</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="63">
+        <v>54599</v>
+      </c>
+      <c r="C6" s="62">
+        <v>8</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+      <c r="F7" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="66" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="63">
+        <v>240</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="64" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="62" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="63">
+        <v>240</v>
+      </c>
+      <c r="H11" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="62" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="69"/>
+      <c r="G20" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F21" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F22" s="69"/>
+      <c r="G22" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F24" s="69"/>
+      <c r="G24" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I25" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="69"/>
+      <c r="G26" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" s="71">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F25:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>